<commit_message>
Modularised word2vec and updated data models and results
</commit_message>
<xml_diff>
--- a/Word2Vec/outputgeneratedw2v.xlsx
+++ b/Word2Vec/outputgeneratedw2v.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -814,11 +814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="184500944"/>
-        <c:axId val="475043360"/>
+        <c:axId val="349483840"/>
+        <c:axId val="349484232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="184500944"/>
+        <c:axId val="349483840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -876,12 +876,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475043360"/>
+        <c:crossAx val="349484232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="475043360"/>
+        <c:axId val="349484232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -939,7 +939,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184500944"/>
+        <c:crossAx val="349483840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1845,7 +1845,7 @@
   <dimension ref="A1:N17327"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="H1" sqref="H1:N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,11 +1909,11 @@
         <v>532</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J12" si="1">COUNTIF(B:B,"&lt;" &amp; H3)</f>
+        <f t="shared" ref="J3:J7" si="1">COUNTIF(B:B,"&lt;" &amp; H3)</f>
         <v>119</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:N19" si="2">J3/J$19</f>
+        <f t="shared" ref="M3:M19" si="2">J3/J$19</f>
         <v>1.558815823945507E-2</v>
       </c>
       <c r="N3">
@@ -2022,11 +2022,11 @@
         <v>0.4</v>
       </c>
       <c r="I8">
-        <f>COUNTIF(A:A,"&lt;" &amp; H8)-F$2</f>
+        <f t="shared" ref="I8:I19" si="4">COUNTIF(A:A,"&lt;" &amp; H8)-F$2</f>
         <v>767</v>
       </c>
       <c r="J8">
-        <f>COUNTIF(B:B,"&lt;" &amp; H8)</f>
+        <f t="shared" ref="J8:J19" si="5">COUNTIF(B:B,"&lt;" &amp; H8)</f>
         <v>426</v>
       </c>
       <c r="M8">
@@ -2049,11 +2049,11 @@
         <v>0.8</v>
       </c>
       <c r="I9">
-        <f>COUNTIF(A:A,"&lt;" &amp; H9)-F$2</f>
+        <f t="shared" si="4"/>
         <v>1419</v>
       </c>
       <c r="J9">
-        <f>COUNTIF(B:B,"&lt;" &amp; H9)</f>
+        <f t="shared" si="5"/>
         <v>911</v>
       </c>
       <c r="M9">
@@ -2070,11 +2070,11 @@
         <v>1.2</v>
       </c>
       <c r="I10">
-        <f>COUNTIF(A:A,"&lt;" &amp; H10)-F$2</f>
+        <f t="shared" si="4"/>
         <v>2388</v>
       </c>
       <c r="J10">
-        <f>COUNTIF(B:B,"&lt;" &amp; H10)</f>
+        <f t="shared" si="5"/>
         <v>1536</v>
       </c>
       <c r="M10">
@@ -2097,11 +2097,11 @@
         <v>1.6</v>
       </c>
       <c r="I11">
-        <f>COUNTIF(A:A,"&lt;" &amp; H11)-F$2</f>
+        <f t="shared" si="4"/>
         <v>3456</v>
       </c>
       <c r="J11">
-        <f>COUNTIF(B:B,"&lt;" &amp; H11)</f>
+        <f t="shared" si="5"/>
         <v>2265</v>
       </c>
       <c r="M11">
@@ -2118,11 +2118,11 @@
         <v>2</v>
       </c>
       <c r="I12">
-        <f>COUNTIF(A:A,"&lt;" &amp; H12)-F$2</f>
+        <f t="shared" si="4"/>
         <v>4327</v>
       </c>
       <c r="J12">
-        <f>COUNTIF(B:B,"&lt;" &amp; H12)</f>
+        <f t="shared" si="5"/>
         <v>2991</v>
       </c>
       <c r="M12">
@@ -2145,11 +2145,11 @@
         <v>2.4</v>
       </c>
       <c r="I13">
-        <f>COUNTIF(A:A,"&lt;" &amp; H13)-F$2</f>
+        <f t="shared" si="4"/>
         <v>5073</v>
       </c>
       <c r="J13">
-        <f>COUNTIF(B:B,"&lt;" &amp; H13)</f>
+        <f t="shared" si="5"/>
         <v>3637</v>
       </c>
       <c r="M13">
@@ -2166,11 +2166,11 @@
         <v>2.8</v>
       </c>
       <c r="I14">
-        <f>COUNTIF(A:A,"&lt;" &amp; H14)-F$2</f>
+        <f t="shared" si="4"/>
         <v>5750</v>
       </c>
       <c r="J14">
-        <f>COUNTIF(B:B,"&lt;" &amp; H14)</f>
+        <f t="shared" si="5"/>
         <v>4235</v>
       </c>
       <c r="M14">
@@ -2193,11 +2193,11 @@
         <v>3.2</v>
       </c>
       <c r="I15">
-        <f>COUNTIF(A:A,"&lt;" &amp; H15)-F$2</f>
+        <f t="shared" si="4"/>
         <v>6262</v>
       </c>
       <c r="J15">
-        <f>COUNTIF(B:B,"&lt;" &amp; H15)</f>
+        <f t="shared" si="5"/>
         <v>4763</v>
       </c>
       <c r="M15">
@@ -2214,11 +2214,11 @@
         <v>6.4</v>
       </c>
       <c r="I16">
-        <f>COUNTIF(A:A,"&lt;" &amp; H16)-F$2</f>
+        <f t="shared" si="4"/>
         <v>8372</v>
       </c>
       <c r="J16">
-        <f>COUNTIF(B:B,"&lt;" &amp; H16)</f>
+        <f t="shared" si="5"/>
         <v>7252</v>
       </c>
       <c r="M16">
@@ -2241,11 +2241,11 @@
         <v>10</v>
       </c>
       <c r="I17">
-        <f>COUNTIF(A:A,"&lt;" &amp; H17)-F$2</f>
+        <f t="shared" si="4"/>
         <v>8645</v>
       </c>
       <c r="J17">
-        <f>COUNTIF(B:B,"&lt;" &amp; H17)</f>
+        <f t="shared" si="5"/>
         <v>7584</v>
       </c>
       <c r="M17">
@@ -2262,11 +2262,11 @@
         <v>15</v>
       </c>
       <c r="I18">
-        <f>COUNTIF(A:A,"&lt;" &amp; H18)-F$2</f>
+        <f t="shared" si="4"/>
         <v>8664</v>
       </c>
       <c r="J18">
-        <f>COUNTIF(B:B,"&lt;" &amp; H18)</f>
+        <f t="shared" si="5"/>
         <v>7629</v>
       </c>
       <c r="M18">
@@ -2289,11 +2289,11 @@
         <v>20</v>
       </c>
       <c r="I19">
-        <f>COUNTIF(A:A,"&lt;" &amp; H19)-F$2</f>
+        <f t="shared" si="4"/>
         <v>8664</v>
       </c>
       <c r="J19">
-        <f>COUNTIF(B:B,"&lt;" &amp; H19)</f>
+        <f t="shared" si="5"/>
         <v>7634</v>
       </c>
       <c r="M19">

</xml_diff>